<commit_message>
Clean-up on macbook :q!
</commit_message>
<xml_diff>
--- a/Tested_Sample.xlsx
+++ b/Tested_Sample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/larawieland/Documents/Promotion/SALAD/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EE495B3-B789-294B-AF8B-187E91A01D3C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E576792B-FCDC-774C-B9FC-CB647002A109}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4680" yWindow="580" windowWidth="28780" windowHeight="16280" xr2:uid="{EF68107C-7A59-4EA7-BD73-84812200EC48}"/>
+    <workbookView xWindow="2800" yWindow="1160" windowWidth="27820" windowHeight="16280" xr2:uid="{EF68107C-7A59-4EA7-BD73-84812200EC48}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,21 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="83">
   <si>
     <t>All</t>
   </si>
@@ -268,13 +277,19 @@
   </si>
   <si>
     <t>behav_out</t>
+  </si>
+  <si>
+    <t>scan artefact</t>
+  </si>
+  <si>
+    <t>mirror</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -311,8 +326,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -334,6 +355,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -425,7 +452,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -451,15 +478,19 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -776,8 +807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E7A23B5-BB81-4D78-BEEA-D748A3DACFDC}">
   <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -801,20 +832,20 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="16"/>
+      <c r="B2" s="23"/>
       <c r="C2" s="6" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="7">
         <v>20</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="16"/>
+      <c r="F2" s="23"/>
       <c r="G2" s="6" t="s">
         <v>4</v>
       </c>
@@ -879,13 +910,13 @@
       <c r="A5">
         <v>1</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="17" t="s">
+      <c r="C5" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="15" t="s">
         <v>80</v>
       </c>
       <c r="E5">
@@ -905,7 +936,7 @@
       <c r="A6">
         <v>2</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="18" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="13" t="s">
@@ -974,7 +1005,7 @@
       <c r="A9">
         <v>5</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="18" t="s">
         <v>18</v>
       </c>
       <c r="C9" s="13" t="s">
@@ -1006,13 +1037,13 @@
       <c r="E10">
         <v>6</v>
       </c>
-      <c r="F10" s="18" t="s">
+      <c r="F10" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="G10" s="18" t="s">
+      <c r="G10" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="I10" s="19" t="s">
+      <c r="I10" s="17" t="s">
         <v>80</v>
       </c>
     </row>
@@ -1020,7 +1051,7 @@
       <c r="A11">
         <v>7</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="18" t="s">
         <v>22</v>
       </c>
       <c r="C11" s="13" t="s">
@@ -1046,7 +1077,7 @@
       <c r="A12">
         <v>8</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="18" t="s">
         <v>24</v>
       </c>
       <c r="C12" s="13" t="s">
@@ -1069,14 +1100,14 @@
       <c r="A13">
         <v>9</v>
       </c>
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="D13" s="17" t="s">
-        <v>80</v>
+      <c r="C13" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="20" t="s">
+        <v>10</v>
       </c>
       <c r="E13">
         <v>9</v>
@@ -1095,7 +1126,7 @@
       <c r="A14">
         <v>10</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="18" t="s">
         <v>28</v>
       </c>
       <c r="C14" s="13" t="s">
@@ -1125,7 +1156,7 @@
         <v>30</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="E15">
         <v>11</v>
@@ -1161,7 +1192,7 @@
       <c r="A17">
         <v>13</v>
       </c>
-      <c r="B17" s="13" t="s">
+      <c r="B17" s="18" t="s">
         <v>34</v>
       </c>
       <c r="C17" s="13" t="s">
@@ -1187,7 +1218,7 @@
       <c r="A18">
         <v>14</v>
       </c>
-      <c r="B18" s="13" t="s">
+      <c r="B18" s="18" t="s">
         <v>37</v>
       </c>
       <c r="C18" s="13" t="s">
@@ -1199,16 +1230,16 @@
       <c r="E18">
         <v>14</v>
       </c>
-      <c r="F18" s="17" t="s">
+      <c r="F18" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="G18" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="H18" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="I18" s="17" t="s">
+      <c r="G18" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="H18" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I18" s="15" t="s">
         <v>80</v>
       </c>
     </row>
@@ -1216,7 +1247,7 @@
       <c r="A19">
         <v>15</v>
       </c>
-      <c r="B19" s="13" t="s">
+      <c r="B19" s="18" t="s">
         <v>39</v>
       </c>
       <c r="C19" s="13" t="s">
@@ -1239,7 +1270,7 @@
       <c r="A20">
         <v>16</v>
       </c>
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="18" t="s">
         <v>41</v>
       </c>
       <c r="C20" s="13" t="s">
@@ -1265,7 +1296,7 @@
       <c r="A21">
         <v>17</v>
       </c>
-      <c r="B21" s="13" t="s">
+      <c r="B21" s="18" t="s">
         <v>43</v>
       </c>
       <c r="C21" s="13" t="s">
@@ -1288,7 +1319,7 @@
       <c r="A22">
         <v>18</v>
       </c>
-      <c r="B22" s="13" t="s">
+      <c r="B22" s="18" t="s">
         <v>45</v>
       </c>
       <c r="C22" s="13" t="s">
@@ -1300,16 +1331,16 @@
       <c r="E22">
         <v>18</v>
       </c>
-      <c r="F22" s="17" t="s">
+      <c r="F22" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="G22" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="H22" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="I22" s="17" t="s">
+      <c r="G22" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="H22" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I22" s="15" t="s">
         <v>80</v>
       </c>
     </row>
@@ -1317,7 +1348,7 @@
       <c r="A23">
         <v>19</v>
       </c>
-      <c r="B23" s="13" t="s">
+      <c r="B23" s="18" t="s">
         <v>47</v>
       </c>
       <c r="C23" s="13" t="s">
@@ -1329,13 +1360,13 @@
       <c r="E23">
         <v>19</v>
       </c>
-      <c r="F23" s="18" t="s">
+      <c r="F23" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="G23" s="18" t="s">
+      <c r="G23" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="I23" s="19" t="s">
+      <c r="I23" s="17" t="s">
         <v>80</v>
       </c>
     </row>
@@ -1343,7 +1374,7 @@
       <c r="A24">
         <v>20</v>
       </c>
-      <c r="B24" s="13" t="s">
+      <c r="B24" s="18" t="s">
         <v>49</v>
       </c>
       <c r="C24" s="13" t="s">
@@ -1366,7 +1397,7 @@
       <c r="A25">
         <v>21</v>
       </c>
-      <c r="B25" s="13" t="s">
+      <c r="B25" s="18" t="s">
         <v>51</v>
       </c>
       <c r="C25" s="13" t="s">
@@ -1392,7 +1423,7 @@
       <c r="A26">
         <v>22</v>
       </c>
-      <c r="B26" s="13" t="s">
+      <c r="B26" s="18" t="s">
         <v>53</v>
       </c>
       <c r="C26" s="13" t="s">
@@ -1418,7 +1449,7 @@
       <c r="A27">
         <v>23</v>
       </c>
-      <c r="B27" s="13" t="s">
+      <c r="B27" s="18" t="s">
         <v>55</v>
       </c>
       <c r="C27" s="13" t="s">
@@ -1430,13 +1461,13 @@
       <c r="E27">
         <v>23</v>
       </c>
-      <c r="F27" s="18" t="s">
+      <c r="F27" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="G27" s="18" t="s">
+      <c r="G27" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="I27" s="19" t="s">
+      <c r="I27" s="17" t="s">
         <v>80</v>
       </c>
     </row>
@@ -1444,7 +1475,7 @@
       <c r="A28">
         <v>24</v>
       </c>
-      <c r="B28" s="13" t="s">
+      <c r="B28" s="18" t="s">
         <v>57</v>
       </c>
       <c r="C28" s="13" t="s">
@@ -1467,7 +1498,7 @@
       <c r="A29">
         <v>25</v>
       </c>
-      <c r="B29" s="13" t="s">
+      <c r="B29" s="18" t="s">
         <v>59</v>
       </c>
       <c r="C29" s="13" t="s">
@@ -1516,7 +1547,7 @@
       <c r="A31">
         <v>27</v>
       </c>
-      <c r="B31" s="13" t="s">
+      <c r="B31" s="18" t="s">
         <v>63</v>
       </c>
       <c r="C31" s="13" t="s">
@@ -1539,7 +1570,7 @@
       <c r="A32">
         <v>28</v>
       </c>
-      <c r="B32" s="13" t="s">
+      <c r="B32" s="18" t="s">
         <v>65</v>
       </c>
       <c r="C32" s="13" t="s">
@@ -1570,7 +1601,7 @@
       <c r="A34">
         <v>30</v>
       </c>
-      <c r="B34" s="13" t="s">
+      <c r="B34" s="18" t="s">
         <v>67</v>
       </c>
       <c r="C34" s="13" t="s">
@@ -1587,7 +1618,7 @@
       <c r="A35">
         <v>31</v>
       </c>
-      <c r="B35" s="13" t="s">
+      <c r="B35" s="18" t="s">
         <v>68</v>
       </c>
       <c r="C35" s="13" t="s">
@@ -1605,14 +1636,14 @@
         <v>69</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>33</v>
       </c>
-      <c r="B37" s="13" t="s">
+      <c r="B37" s="18" t="s">
         <v>70</v>
       </c>
       <c r="C37" s="13" t="s">
@@ -1626,7 +1657,7 @@
       <c r="A38">
         <v>34</v>
       </c>
-      <c r="B38" s="13" t="s">
+      <c r="B38" s="18" t="s">
         <v>71</v>
       </c>
       <c r="C38" s="13" t="s">
@@ -1640,7 +1671,7 @@
       <c r="A39">
         <v>35</v>
       </c>
-      <c r="B39" s="13" t="s">
+      <c r="B39" s="18" t="s">
         <v>72</v>
       </c>
       <c r="C39" s="13" t="s">
@@ -1665,7 +1696,7 @@
       <c r="A41">
         <v>37</v>
       </c>
-      <c r="B41" s="13" t="s">
+      <c r="B41" s="18" t="s">
         <v>74</v>
       </c>
       <c r="C41" s="13" t="s">
@@ -1679,7 +1710,7 @@
       <c r="A42">
         <v>38</v>
       </c>
-      <c r="B42" s="13" t="s">
+      <c r="B42" s="18" t="s">
         <v>75</v>
       </c>
       <c r="C42" s="13" t="s">

</xml_diff>